<commit_message>
fixed fy/calendar issue + formatting
 - changed from Fiscal Year + date to just using one input.
 - also added consistency throughout in variable names. Changed the excel files to reflect this
</commit_message>
<xml_diff>
--- a/data/Indicators_Targets.xlsx
+++ b/data/Indicators_Targets.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryo Nakagawara\Documents\R_materials\AV.BulletChart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\Dropbox\My projects\bulletchartr\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13425" windowHeight="5850"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="13428" windowHeight="5856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,18 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>IndicatorName</t>
-  </si>
-  <si>
-    <t>Actual</t>
-  </si>
-  <si>
-    <t>Actual_lastWeek</t>
-  </si>
-  <si>
-    <t>Actual_lastYear</t>
-  </si>
-  <si>
     <t>Ind 04</t>
   </si>
   <si>
@@ -56,13 +44,25 @@
     <t>Ind 18</t>
   </si>
   <si>
-    <t>Target</t>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>actual_lastweek</t>
+  </si>
+  <si>
+    <t>actual_lastyear</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>indicator_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,31 +376,31 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -415,9 +415,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>437</v>
@@ -432,9 +432,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -449,9 +449,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>44</v>
@@ -466,9 +466,9 @@
         <v>10327</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -483,9 +483,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>10000</v>

</xml_diff>